<commit_message>
Fix: Update map with corrected coordinates and exclude specific DCUs
</commit_message>
<xml_diff>
--- a/public/data/DCUS.xlsx
+++ b/public/data/DCUS.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nansencombr-my.sharepoint.com/personal/graziele_souza_nansen_com_br/Documents/Dashboards/I-NOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A0EC5FB7-D927-40CD-87E6-671446261979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41B9D180-43A7-45DE-A84F-84929C5FBEF1}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{A0EC5FB7-D927-40CD-87E6-671446261979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2735C35A-6B8A-44DC-8D9C-BC52D9BE20EA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{97B31D7E-D4FC-4B15-8794-1B701CB06B31}"/>
+    <workbookView xWindow="-19290" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{97B31D7E-D4FC-4B15-8794-1B701CB06B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$L$819</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -7786,7 +7789,7 @@
   <dimension ref="A1:L819"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8476,10 +8479,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>871</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>872</v>
       </c>
       <c r="E20" s="2">
         <v>746</v>
@@ -32739,10 +32742,10 @@
         <v>7</v>
       </c>
       <c r="C708" s="2" t="s">
+        <v>2234</v>
+      </c>
+      <c r="D708" s="2" t="s">
         <v>2233</v>
-      </c>
-      <c r="D708" s="2" t="s">
-        <v>2234</v>
       </c>
       <c r="E708" s="2">
         <v>598</v>
@@ -34653,10 +34656,10 @@
         <v>7</v>
       </c>
       <c r="C762" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="D762" s="2" t="s">
         <v>2336</v>
-      </c>
-      <c r="D762" s="2" t="s">
-        <v>2337</v>
       </c>
       <c r="E762" s="2">
         <v>935</v>
@@ -36715,6 +36718,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L819" xr:uid="{68203FA2-659E-4072-9F6D-D3DE6A59D2BF}"/>
   <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="containsText" dxfId="0" priority="33" operator="containsText" text="Offline">
       <formula>NOT(ISERROR(SEARCH("Offline",B1)))</formula>
@@ -36905,7 +36909,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J801:K819">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="500"/>
@@ -36915,7 +36919,7 @@
         <color rgb="FFFF7C80"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="500"/>
@@ -36967,7 +36971,7 @@
         <color rgb="FFFF7C80"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="500"/>
@@ -36977,7 +36981,7 @@
         <color rgb="FFFF7C80"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="500"/>
@@ -36990,16 +36994,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K819">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="500"/>
-        <cfvo type="num" val="1000"/>
-        <color theme="9" tint="0.59999389629810485"/>
-        <color theme="7" tint="0.79998168889431442"/>
-        <color rgb="FFFF7C80"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="500"/>
@@ -37029,8 +37023,38 @@
         <color rgb="FFFF7C80"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="500"/>
+        <cfvo type="num" val="1000"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color rgb="FFFF7C80"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K801:K819">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="500"/>
+        <cfvo type="num" val="1000"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color rgb="FFFF7C80"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="500"/>
+        <cfvo type="num" val="1000"/>
+        <color theme="9" tint="0.59999389629810485"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color rgb="FFFF7C80"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -37091,26 +37115,6 @@
         <color rgb="FFFF7C80"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="500"/>
-        <cfvo type="num" val="1000"/>
-        <color theme="9" tint="0.59999389629810485"/>
-        <color theme="7" tint="0.79998168889431442"/>
-        <color rgb="FFFF7C80"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="500"/>
-        <cfvo type="num" val="1000"/>
-        <color theme="9" tint="0.59999389629810485"/>
-        <color theme="7" tint="0.79998168889431442"/>
-        <color rgb="FFFF7C80"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
     <cfRule type="colorScale" priority="39">

</xml_diff>